<commit_message>
fix bug tamplate 1.2
</commit_message>
<xml_diff>
--- a/tamplate.xlsx
+++ b/tamplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asman\Desktop\SkripsiProgram\programSkripsi1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F8D11-52A0-4AA1-BD3F-96C3D97729C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D476498C-E809-4D7A-B3DC-4E3A3235AA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{28874C38-D82B-4CE7-AA47-1DAFC7AE77C5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="merek" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transaksi!$A$1:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transaksi!$A$1:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,13 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Tanggal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>banyak</t>
   </si>
@@ -226,6 +220,9 @@
   </si>
   <si>
     <t>QueenMask Earloop Hitam</t>
+  </si>
+  <si>
+    <t>tanggal</t>
   </si>
 </sst>
 </file>
@@ -595,85 +592,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232DF459-3AC5-498A-8893-2C034DD0899B}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -684,7 +678,7 @@
           <x14:formula1>
             <xm:f>merek!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -714,411 +708,411 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="6"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="6"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="6"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="6"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="6"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C28" s="6"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" s="6"/>
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="6"/>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="6"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="6"/>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="6"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C34" s="6"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="6"/>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="6"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="6"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="6"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="6"/>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="6"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="6"/>
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42" s="6"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43" s="6"/>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="6"/>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" s="6"/>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="6"/>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C47" s="6"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C48" s="6"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C49" s="6"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C50" s="6"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51" s="6"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" s="6"/>
       <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C53" s="6"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C54" s="6"/>
       <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C55" s="6"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6"/>
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C57" s="6"/>
       <c r="E57" s="6"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C58" s="6"/>
       <c r="E58" s="6"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C59" s="6"/>
       <c r="E59" s="6"/>

</xml_diff>